<commit_message>
15° Commit: Tabelle, sottoprogrammi, ws per gestione Demo e Reset password
</commit_message>
<xml_diff>
--- a/table/tableList_appCore.xlsx
+++ b/table/tableList_appCore.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorbara\Documents\ArgoX3_API_Mobile_CORE\table\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D61BBB-7DCA-46DF-B8B7-B4B39643D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle" sheetId="1" r:id="rId1"/>
+    <sheet name="Campi di Tabella" sheetId="2" r:id="rId2"/>
+    <sheet name="Indici" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +26,125 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+  <si>
+    <t xml:space="preserve">Codice </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbr </t>
+  </si>
+  <si>
+    <t>Descrizione</t>
+  </si>
+  <si>
+    <t>Cod Att</t>
+  </si>
+  <si>
+    <t>Modulo</t>
+  </si>
+  <si>
+    <t>Tipo DB</t>
+  </si>
+  <si>
+    <t>Tipo Tabella</t>
+  </si>
+  <si>
+    <t>Cod Indice</t>
+  </si>
+  <si>
+    <t>Descr Indice</t>
+  </si>
+  <si>
+    <t>Omonimi</t>
+  </si>
+  <si>
+    <t>Patch</t>
+  </si>
+  <si>
+    <t>YAX3MDEMOINF</t>
+  </si>
+  <si>
+    <t>YAX3MDI</t>
+  </si>
+  <si>
+    <t>Richiesta informazioni demo</t>
+  </si>
+  <si>
+    <t>YAX3C</t>
+  </si>
+  <si>
+    <t>Supervisore</t>
+  </si>
+  <si>
+    <t>Dossier</t>
+  </si>
+  <si>
+    <t>Applicativa</t>
+  </si>
+  <si>
+    <t>YAX3MDI0</t>
+  </si>
+  <si>
+    <t>AUUID</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Tabella</t>
+  </si>
+  <si>
+    <t>Colonna (campo)</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Menù</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>Att</t>
+  </si>
+  <si>
+    <t>Dim</t>
+  </si>
+  <si>
+    <t>Obblig</t>
+  </si>
+  <si>
+    <t>Opzioni</t>
+  </si>
+  <si>
+    <t>Tabella Collegata</t>
+  </si>
+  <si>
+    <t>cancellazione</t>
+  </si>
+  <si>
+    <t>Descr Normale</t>
+  </si>
+  <si>
+    <t>Descr breve</t>
+  </si>
+  <si>
+    <t>Descr Lunga</t>
+  </si>
+  <si>
+    <t>Codice Indice</t>
+  </si>
+  <si>
+    <t>Descrizione Indice</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +152,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,15 +183,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +565,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D8656-12D3-424C-8502-8CAC1257836B}">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EFA61F-EFB2-4DF1-B048-E40FD10682D3}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>